<commit_message>
ADD: STM32F051 dev board PCB list entry and invoice
</commit_message>
<xml_diff>
--- a/Documents/Material/Zephyrus Shopping List.xlsx
+++ b/Documents/Material/Zephyrus Shopping List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repo\school\4th year\Project 1\Repository\zephyrus\Documents\Material\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F206E7C-86F4-463D-9252-6BB7C43DDCB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{670C19D7-C15A-4C33-8143-572B09E59F08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4290" yWindow="3120" windowWidth="27930" windowHeight="11775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2445" yWindow="3120" windowWidth="27930" windowHeight="11775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -61,6 +61,12 @@
   </si>
   <si>
     <t>Robot platform</t>
+  </si>
+  <si>
+    <t>STM32F051 dev board PCB</t>
+  </si>
+  <si>
+    <t>JLCPCB</t>
   </si>
 </sst>
 </file>
@@ -104,7 +110,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -114,6 +120,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -405,7 +414,7 @@
   <dimension ref="B3:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -443,7 +452,7 @@
       <c r="J3" s="1"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="5">
+      <c r="B4" s="6">
         <v>44138</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -455,18 +464,18 @@
       <c r="E4" s="4">
         <v>3</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="7">
         <v>0</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="5"/>
+      <c r="B5" s="6"/>
       <c r="C5" s="4" t="s">
         <v>7</v>
       </c>
@@ -476,9 +485,9 @@
       <c r="E5" s="4">
         <v>9.8000000000000007</v>
       </c>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
@@ -504,13 +513,27 @@
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
+      <c r="B7" s="5">
+        <v>44158</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="4">
+        <v>1</v>
+      </c>
+      <c r="E7" s="4">
+        <v>16.260000000000002</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="4">
+        <v>0</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="4"/>

</xml_diff>

<commit_message>
UPDT: Low Battery check routine working on remote system working
</commit_message>
<xml_diff>
--- a/Documents/Material/Zephyrus Shopping List.xlsx
+++ b/Documents/Material/Zephyrus Shopping List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repo\school\4th year\Project 1\Repository\zephyrus\Documents\Material\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{680B209B-1BFE-4CAB-987E-C7EC3C351D88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{256BD8DB-8CDE-4E6E-A166-DAC82E1D8723}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3150" yWindow="2235" windowWidth="15405" windowHeight="11775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10245" yWindow="1515" windowWidth="20370" windowHeight="11775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
   <si>
     <t>Date</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>Mouser</t>
+  </si>
+  <si>
+    <t>nRF24L01+ and nRF24L01+ module adapter</t>
   </si>
 </sst>
 </file>
@@ -125,7 +128,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -141,6 +144,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -429,16 +438,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:J28"/>
+  <dimension ref="B3:J35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="3" max="3" width="32" customWidth="1"/>
+    <col min="3" max="3" width="38.7109375" customWidth="1"/>
     <col min="5" max="5" width="12.7109375" customWidth="1"/>
     <col min="6" max="6" width="13.85546875" customWidth="1"/>
     <col min="7" max="7" width="19.28515625" customWidth="1"/>
@@ -470,7 +479,7 @@
       <c r="J3" s="1"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="7">
+      <c r="B4" s="9">
         <v>44138</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -482,18 +491,18 @@
       <c r="E4" s="4">
         <v>3</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="10">
         <v>0</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="H4" s="10" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="7"/>
+      <c r="B5" s="9"/>
       <c r="C5" s="4" t="s">
         <v>7</v>
       </c>
@@ -503,9 +512,9 @@
       <c r="E5" s="4">
         <v>9.8000000000000007</v>
       </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
@@ -623,13 +632,27 @@
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
+      <c r="B11" s="7">
+        <v>44194</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="4">
+        <v>2</v>
+      </c>
+      <c r="E11" s="4">
+        <v>10</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="4">
+        <v>0</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" s="4"/>
@@ -714,7 +737,6 @@
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
@@ -723,7 +745,6 @@
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
@@ -732,7 +753,6 @@
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
@@ -741,48 +761,54 @@
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
       <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
       <c r="H27" s="4"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G29" s="4"/>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G30" s="4"/>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G31" s="4"/>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G32" s="4"/>
+    </row>
+    <row r="33" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="G33" s="4"/>
+    </row>
+    <row r="34" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="G34" s="4"/>
+    </row>
+    <row r="35" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C35" s="4"/>
+      <c r="G35" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
Project at the time of delivery
</commit_message>
<xml_diff>
--- a/Documents/Material/Zephyrus Shopping List.xlsx
+++ b/Documents/Material/Zephyrus Shopping List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repo\school\4th year\Project 1\Repository\zephyrus\Documents\Material\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{256BD8DB-8CDE-4E6E-A166-DAC82E1D8723}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94C5FDA8-C0A3-4465-8485-82982D374C68}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10245" yWindow="1515" windowWidth="20370" windowHeight="11775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14235" yWindow="0" windowWidth="21375" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
   <si>
     <t>Date</t>
   </si>
@@ -55,9 +55,6 @@
   </si>
   <si>
     <t>bot'n'roll</t>
-  </si>
-  <si>
-    <t>JM</t>
   </si>
   <si>
     <t>Robot platform</t>
@@ -441,7 +438,7 @@
   <dimension ref="B3:J35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,7 +495,7 @@
         <v>0</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
@@ -521,7 +518,7 @@
         <v>44140</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D6" s="4">
         <v>1</v>
@@ -536,7 +533,7 @@
         <v>0</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
@@ -544,7 +541,7 @@
         <v>44158</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D7" s="4">
         <v>1</v>
@@ -553,13 +550,13 @@
         <v>2.11</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G7" s="4">
         <v>14.15</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
@@ -567,10 +564,10 @@
         <v>44168</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E8" s="4">
         <v>32.75</v>
@@ -582,7 +579,7 @@
         <v>0</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
@@ -590,22 +587,22 @@
         <v>44187</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E9" s="4">
         <v>6.54</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G9" s="4">
         <v>12.09</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
@@ -613,22 +610,22 @@
         <v>44187</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E10" s="4">
         <v>66.75</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G10" s="4">
         <v>0</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
@@ -636,7 +633,7 @@
         <v>44194</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D11" s="4">
         <v>2</v>
@@ -651,7 +648,7 @@
         <v>0</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">

</xml_diff>